<commit_message>
Fixes some Excel formatting
</commit_message>
<xml_diff>
--- a/Ryan Mann Domain Model.xlsx
+++ b/Ryan Mann Domain Model.xlsx
@@ -74,9 +74,6 @@
     <t>Mann</t>
   </si>
   <si>
-    <t>Monday11</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -375,6 +372,9 @@
   </si>
   <si>
     <t>timeslot 30 taken by interview preppee</t>
+  </si>
+  <si>
+    <t>AppCreator</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <dimension ref="A1:BT48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,9 +736,13 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="40" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="40" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="41" max="49" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="70" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="71" max="72" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72" x14ac:dyDescent="0.3">
@@ -779,10 +783,10 @@
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:72" x14ac:dyDescent="0.3">
@@ -790,16 +794,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:72" x14ac:dyDescent="0.3">
@@ -807,16 +811,16 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:72" x14ac:dyDescent="0.3">
@@ -841,199 +845,199 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" t="s">
         <v>57</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>58</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>59</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>60</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>61</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>62</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>63</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>64</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>65</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>66</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>67</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>68</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>69</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>70</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>71</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>72</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>73</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>74</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>75</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>76</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>77</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AG9" t="s">
         <v>78</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AH9" t="s">
         <v>79</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AI9" t="s">
         <v>80</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AJ9" t="s">
         <v>81</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AK9" t="s">
         <v>82</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AL9" t="s">
         <v>83</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AM9" t="s">
         <v>84</v>
       </c>
-      <c r="AM9" t="s">
+      <c r="AN9" t="s">
         <v>85</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AO9" t="s">
         <v>86</v>
       </c>
-      <c r="AO9" t="s">
+      <c r="AP9" t="s">
         <v>87</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AQ9" t="s">
         <v>88</v>
       </c>
-      <c r="AQ9" t="s">
+      <c r="AR9" t="s">
         <v>89</v>
       </c>
-      <c r="AR9" t="s">
+      <c r="AS9" t="s">
         <v>90</v>
       </c>
-      <c r="AS9" t="s">
+      <c r="AT9" t="s">
         <v>91</v>
       </c>
-      <c r="AT9" t="s">
+      <c r="AU9" t="s">
         <v>92</v>
       </c>
-      <c r="AU9" t="s">
+      <c r="AV9" t="s">
         <v>93</v>
       </c>
-      <c r="AV9" t="s">
+      <c r="AW9" t="s">
         <v>94</v>
       </c>
-      <c r="AW9" t="s">
+      <c r="AX9" t="s">
         <v>95</v>
       </c>
-      <c r="AX9" t="s">
+      <c r="AY9" t="s">
         <v>96</v>
       </c>
-      <c r="AY9" t="s">
+      <c r="AZ9" t="s">
         <v>97</v>
       </c>
-      <c r="AZ9" t="s">
+      <c r="BA9" t="s">
         <v>98</v>
       </c>
-      <c r="BA9" t="s">
+      <c r="BB9" t="s">
         <v>99</v>
       </c>
-      <c r="BB9" t="s">
+      <c r="BC9" t="s">
         <v>100</v>
       </c>
-      <c r="BC9" t="s">
+      <c r="BD9" t="s">
         <v>101</v>
       </c>
-      <c r="BD9" t="s">
+      <c r="BE9" t="s">
         <v>102</v>
       </c>
-      <c r="BE9" t="s">
+      <c r="BF9" t="s">
         <v>103</v>
       </c>
-      <c r="BF9" t="s">
+      <c r="BG9" t="s">
         <v>104</v>
       </c>
-      <c r="BG9" t="s">
+      <c r="BH9" t="s">
         <v>105</v>
       </c>
-      <c r="BH9" t="s">
+      <c r="BI9" t="s">
         <v>106</v>
       </c>
-      <c r="BI9" t="s">
+      <c r="BJ9" t="s">
         <v>107</v>
       </c>
-      <c r="BJ9" t="s">
+      <c r="BK9" t="s">
         <v>108</v>
       </c>
-      <c r="BK9" t="s">
+      <c r="BL9" t="s">
         <v>109</v>
       </c>
-      <c r="BL9" t="s">
+      <c r="BM9" t="s">
         <v>110</v>
       </c>
-      <c r="BM9" t="s">
+      <c r="BN9" t="s">
         <v>111</v>
       </c>
-      <c r="BN9" t="s">
+      <c r="BO9" t="s">
         <v>112</v>
       </c>
-      <c r="BO9" t="s">
+      <c r="BP9" t="s">
         <v>113</v>
       </c>
-      <c r="BP9" t="s">
+      <c r="BQ9" t="s">
         <v>114</v>
       </c>
-      <c r="BQ9" t="s">
+      <c r="BR9" t="s">
         <v>115</v>
-      </c>
-      <c r="BR9" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:72" x14ac:dyDescent="0.3">
@@ -1041,16 +1045,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1259,16 +1263,16 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -1319,61 +1323,61 @@
         <v>52</v>
       </c>
       <c r="V11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AA11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AB11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AD11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AF11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AH11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AI11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AJ11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AK11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AL11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AM11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AN11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AO11">
         <v>60</v>
@@ -1409,67 +1413,67 @@
         <v>1</v>
       </c>
       <c r="AZ11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BA11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BB11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BC11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BD11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BE11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BF11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BG11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BH11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BI11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BJ11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BK11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BL11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BM11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BN11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BO11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BP11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BQ11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BR11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BS11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BT11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.3">
@@ -1477,16 +1481,16 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -1495,13 +1499,13 @@
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K12">
         <v>60</v>
@@ -1714,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1725,7 +1729,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1736,12 +1740,12 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1757,7 +1761,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1765,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1773,7 +1777,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1786,7 +1790,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -1839,7 +1843,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1847,7 +1851,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1855,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1863,7 +1867,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -1871,12 +1875,12 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1892,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1900,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1908,12 +1912,12 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>